<commit_message>
Updated analysis dataset, corrected few mistakes and added indicator variables for sensitivity analyses using last registry and midpoint
</commit_message>
<xml_diff>
--- a/input/20220120-study.characteristics_update.xlsx
+++ b/input/20220120-study.characteristics_update.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\SR_prevalence_NTM\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96C8A0E-0556-414F-AB08-5705884CB5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4549D0D-F9FB-49B7-9E2F-AF762C37BC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{9BAFF895-4EE1-48C5-B0C9-C001584A386E}"/>
   </bookViews>
@@ -21047,9 +21047,6 @@
 M. malmoense - 1</t>
   </si>
   <si>
-    <t>14 / 376 (3.76%)</t>
-  </si>
-  <si>
     <t>1989 - 1997?</t>
   </si>
   <si>
@@ -22535,9 +22532,6 @@
     <t xml:space="preserve"> establish  NTM prevalence and treatment success in children with CF, and to identify any factors that may affect treatment success.</t>
   </si>
   <si>
-    <t>40/59 - 67.8%</t>
-  </si>
-  <si>
     <t>Described only the 
 Z-scores</t>
   </si>
@@ -22838,6 +22832,13 @@
 ≥40 &amp; &lt;70 - 630 (28.5)
 &lt;40 - 227 (10.3)</t>
     </r>
+  </si>
+  <si>
+    <t>14 / 372 (3.76%)</t>
+  </si>
+  <si>
+    <t>NTM +
+40/63 - 63.5%</t>
   </si>
 </sst>
 </file>
@@ -23380,8 +23381,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF44B60-E10E-47AB-8924-A521697E3CBB}">
   <dimension ref="A1:AZ96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15"/>
@@ -23429,7 +23431,7 @@
   <sheetData>
     <row r="1" spans="1:52" ht="20.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
@@ -23558,36 +23560,36 @@
         <v>78</v>
       </c>
       <c r="AR1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>1441</v>
+      </c>
+      <c r="AT1" t="s">
         <v>1442</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>1443</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>1444</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>1445</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>1446</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>1447</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>1448</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>1449</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>1450</v>
       </c>
     </row>
     <row r="2" spans="1:52" ht="158.25" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>147</v>
@@ -23716,22 +23718,22 @@
         <v>46</v>
       </c>
       <c r="AR2" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS2" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT2" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU2" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV2" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW2" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX2">
         <v>4687</v>
@@ -23745,10 +23747,10 @@
     </row>
     <row r="3" spans="1:52" ht="120">
       <c r="A3" s="22" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1359</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1360</v>
       </c>
       <c r="C3" s="2">
         <v>2021</v>
@@ -23757,13 +23759,13 @@
         <v>236</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="F3" s="2">
         <v>485</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>31</v>
@@ -23772,34 +23774,34 @@
         <v>67</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>180</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>110</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>1408</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>1407</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>1409</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>1408</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>1361</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>1410</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>1362</v>
       </c>
       <c r="T3" s="2" t="s">
         <v>322</v>
@@ -23820,76 +23822,76 @@
         <v>46</v>
       </c>
       <c r="Z3" s="2" t="s">
+        <v>1362</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>1363</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="19" t="s">
+        <v>1375</v>
+      </c>
+      <c r="AC3" s="19" t="s">
+        <v>1374</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>1365</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH3" s="3" t="s">
         <v>1364</v>
       </c>
-      <c r="AB3" s="19" t="s">
-        <v>1376</v>
-      </c>
-      <c r="AC3" s="19" t="s">
-        <v>1375</v>
-      </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AI3" s="18" t="s">
+        <v>1410</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
         <v>1366</v>
       </c>
-      <c r="AE3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>1365</v>
-      </c>
-      <c r="AI3" s="18" t="s">
-        <v>1411</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>1368</v>
+      </c>
+      <c r="AO3" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP3" s="2" t="s">
         <v>1367</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN3" s="2" t="s">
-        <v>1369</v>
-      </c>
-      <c r="AO3" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP3" s="2" t="s">
-        <v>1368</v>
       </c>
       <c r="AQ3" s="2">
         <v>0</v>
       </c>
       <c r="AR3" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS3" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT3" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU3" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV3" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW3" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX3">
         <v>485</v>
@@ -23903,7 +23905,7 @@
     </row>
     <row r="4" spans="1:52" ht="269.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>164</v>
@@ -24032,22 +24034,22 @@
         <v>46</v>
       </c>
       <c r="AR4" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS4" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT4" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU4" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV4" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW4" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX4">
         <v>10527</v>
@@ -24061,7 +24063,7 @@
     </row>
     <row r="5" spans="1:52" ht="240">
       <c r="A5" s="1" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>177</v>
@@ -24190,22 +24192,22 @@
         <v>191</v>
       </c>
       <c r="AR5" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS5" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT5" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU5" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV5" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW5" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX5">
         <v>16153</v>
@@ -24219,7 +24221,7 @@
     </row>
     <row r="6" spans="1:52" ht="90">
       <c r="A6" s="1" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
@@ -24348,22 +24350,22 @@
         <v>46</v>
       </c>
       <c r="AR6" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS6" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT6" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU6" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV6" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW6" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX6">
         <v>42</v>
@@ -24377,7 +24379,7 @@
     </row>
     <row r="7" spans="1:52" ht="105">
       <c r="A7" s="17" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>127</v>
@@ -24416,7 +24418,7 @@
         <v>46</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>134</v>
@@ -24482,7 +24484,7 @@
         <v>46</v>
       </c>
       <c r="AJ7" s="2" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>46</v>
@@ -24506,22 +24508,22 @@
         <v>146</v>
       </c>
       <c r="AR7" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX7">
         <v>117</v>
@@ -24535,7 +24537,7 @@
     </row>
     <row r="8" spans="1:52" ht="150">
       <c r="A8" s="1" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>223</v>
@@ -24664,22 +24666,22 @@
         <v>46</v>
       </c>
       <c r="AR8" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS8" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT8" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU8" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV8" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW8" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX8">
         <v>64</v>
@@ -24693,7 +24695,7 @@
     </row>
     <row r="9" spans="1:52" ht="150">
       <c r="A9" s="1" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>749</v>
@@ -24783,7 +24785,7 @@
         <v>46</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>46</v>
@@ -24822,22 +24824,22 @@
         <v>762</v>
       </c>
       <c r="AR9" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS9" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT9" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU9" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV9" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW9" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX9" t="s">
         <v>46</v>
@@ -24851,7 +24853,7 @@
     </row>
     <row r="10" spans="1:52" ht="165">
       <c r="A10" s="1" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>763</v>
@@ -24899,7 +24901,7 @@
         <v>46</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>769</v>
@@ -24980,22 +24982,22 @@
         <v>774</v>
       </c>
       <c r="AR10" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS10" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT10" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU10" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV10" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW10" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX10" t="s">
         <v>46</v>
@@ -25009,7 +25011,7 @@
     </row>
     <row r="11" spans="1:52" ht="180">
       <c r="A11" s="1" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>775</v>
@@ -25138,22 +25140,22 @@
         <v>788</v>
       </c>
       <c r="AR11" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS11" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT11" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU11" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV11" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW11" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX11" t="s">
         <v>46</v>
@@ -25167,7 +25169,7 @@
     </row>
     <row r="12" spans="1:52" ht="225">
       <c r="A12" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>789</v>
@@ -25296,22 +25298,22 @@
         <v>801</v>
       </c>
       <c r="AR12" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS12" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT12" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU12" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV12" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW12" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX12" t="s">
         <v>46</v>
@@ -25325,7 +25327,7 @@
     </row>
     <row r="13" spans="1:52" ht="240">
       <c r="A13" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>802</v>
@@ -25367,7 +25369,7 @@
         <v>805</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="P13" s="2" t="s">
         <v>46</v>
@@ -25454,22 +25456,22 @@
         <v>813</v>
       </c>
       <c r="AR13" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS13" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT13" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU13" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV13" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW13" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX13" t="s">
         <v>46</v>
@@ -25483,7 +25485,7 @@
     </row>
     <row r="14" spans="1:52" ht="240">
       <c r="A14" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>802</v>
@@ -25525,7 +25527,7 @@
         <v>816</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>46</v>
@@ -25612,22 +25614,22 @@
         <v>824</v>
       </c>
       <c r="AR14" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS14" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT14" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU14" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV14" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW14" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX14" t="s">
         <v>46</v>
@@ -25641,7 +25643,7 @@
     </row>
     <row r="15" spans="1:52" ht="240">
       <c r="A15" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>825</v>
@@ -25683,7 +25685,7 @@
         <v>805</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>46</v>
@@ -25770,22 +25772,22 @@
         <v>835</v>
       </c>
       <c r="AR15" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS15" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT15" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU15" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV15" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW15" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX15" t="s">
         <v>46</v>
@@ -25799,7 +25801,7 @@
     </row>
     <row r="16" spans="1:52" ht="240">
       <c r="A16" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>836</v>
@@ -25928,22 +25930,22 @@
         <v>847</v>
       </c>
       <c r="AR16" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS16" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT16" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU16" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV16" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW16" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX16" t="s">
         <v>46</v>
@@ -25957,7 +25959,7 @@
     </row>
     <row r="17" spans="1:52" ht="60">
       <c r="A17" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>1207</v>
@@ -26086,22 +26088,22 @@
         <v>46</v>
       </c>
       <c r="AR17" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS17" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT17" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU17" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV17" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW17" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX17">
         <v>214</v>
@@ -26115,7 +26117,7 @@
     </row>
     <row r="18" spans="1:52" ht="270">
       <c r="A18" s="17" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>235</v>
@@ -26208,7 +26210,7 @@
         <v>253</v>
       </c>
       <c r="AF18" s="13" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="AG18" s="2" t="s">
         <v>255</v>
@@ -26217,7 +26219,7 @@
         <v>256</v>
       </c>
       <c r="AI18" s="14" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="AJ18" s="2" t="s">
         <v>257</v>
@@ -26244,22 +26246,22 @@
         <v>261</v>
       </c>
       <c r="AR18" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS18" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT18" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AU18" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AV18" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW18" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX18">
         <v>180</v>
@@ -26273,7 +26275,7 @@
     </row>
     <row r="19" spans="1:52" ht="180">
       <c r="A19" s="1" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>262</v>
@@ -26387,7 +26389,7 @@
         <v>46</v>
       </c>
       <c r="AM19" s="2" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="AN19" s="2" t="s">
         <v>46</v>
@@ -26402,22 +26404,22 @@
         <v>46</v>
       </c>
       <c r="AR19" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS19" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT19" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU19" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AV19" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW19" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX19" t="s">
         <v>46</v>
@@ -26431,7 +26433,7 @@
     </row>
     <row r="20" spans="1:52" ht="120">
       <c r="A20" s="1" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>850</v>
@@ -26560,22 +26562,22 @@
         <v>863</v>
       </c>
       <c r="AR20" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS20" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT20" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU20" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV20" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW20" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX20" t="s">
         <v>46</v>
@@ -26589,7 +26591,7 @@
     </row>
     <row r="21" spans="1:52" ht="120">
       <c r="A21" s="1" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>864</v>
@@ -26718,22 +26720,22 @@
         <v>863</v>
       </c>
       <c r="AR21" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS21" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT21" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU21" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV21" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW21" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX21" t="s">
         <v>46</v>
@@ -26747,7 +26749,7 @@
     </row>
     <row r="22" spans="1:52" ht="165">
       <c r="A22" s="1" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>874</v>
@@ -26876,22 +26878,22 @@
         <v>876</v>
       </c>
       <c r="AR22" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS22" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT22" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU22" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV22" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW22" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX22" t="s">
         <v>46</v>
@@ -26905,7 +26907,7 @@
     </row>
     <row r="23" spans="1:52" ht="210">
       <c r="A23" s="1" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>888</v>
@@ -27034,22 +27036,22 @@
         <v>898</v>
       </c>
       <c r="AR23" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS23" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT23" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU23" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV23" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW23" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX23" t="s">
         <v>46</v>
@@ -27063,7 +27065,7 @@
     </row>
     <row r="24" spans="1:52" ht="195">
       <c r="A24" s="1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>901</v>
@@ -27192,22 +27194,22 @@
         <v>910</v>
       </c>
       <c r="AR24" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS24" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT24" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU24" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV24" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW24" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX24" t="s">
         <v>46</v>
@@ -27221,7 +27223,7 @@
     </row>
     <row r="25" spans="1:52" ht="180">
       <c r="A25" s="1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>913</v>
@@ -27350,22 +27352,22 @@
         <v>923</v>
       </c>
       <c r="AR25" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS25" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT25" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU25" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV25" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW25" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX25" t="s">
         <v>46</v>
@@ -27379,7 +27381,7 @@
     </row>
     <row r="26" spans="1:52" ht="150">
       <c r="A26" s="1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>926</v>
@@ -27508,22 +27510,22 @@
         <v>936</v>
       </c>
       <c r="AR26" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS26" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT26" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU26" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV26" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW26" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX26" t="s">
         <v>46</v>
@@ -27537,7 +27539,7 @@
     </row>
     <row r="27" spans="1:52" ht="165">
       <c r="A27" s="1" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>939</v>
@@ -27666,22 +27668,22 @@
         <v>950</v>
       </c>
       <c r="AR27" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS27" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT27" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU27" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV27" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW27" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX27" t="s">
         <v>46</v>
@@ -27695,7 +27697,7 @@
     </row>
     <row r="28" spans="1:52" ht="330">
       <c r="A28" s="1" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>276</v>
@@ -27824,22 +27826,22 @@
         <v>46</v>
       </c>
       <c r="AR28" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS28" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT28" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU28" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AV28" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW28" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX28">
         <v>44</v>
@@ -27853,7 +27855,7 @@
     </row>
     <row r="29" spans="1:52" ht="105">
       <c r="A29" s="1" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>952</v>
@@ -27982,22 +27984,22 @@
         <v>46</v>
       </c>
       <c r="AR29" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS29" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT29" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU29" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV29" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW29" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX29" t="s">
         <v>46</v>
@@ -28011,7 +28013,7 @@
     </row>
     <row r="30" spans="1:52" ht="195">
       <c r="A30" s="1" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>953</v>
@@ -28026,7 +28028,7 @@
         <v>956</v>
       </c>
       <c r="F30" s="2">
-        <v>3913</v>
+        <v>3975</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>632</v>
@@ -28140,22 +28142,22 @@
         <v>46</v>
       </c>
       <c r="AR30" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS30" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT30" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU30" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV30" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW30" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX30" t="s">
         <v>46</v>
@@ -28169,7 +28171,7 @@
     </row>
     <row r="31" spans="1:52" ht="195">
       <c r="A31" s="1" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>954</v>
@@ -28298,22 +28300,22 @@
         <v>46</v>
       </c>
       <c r="AR31" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS31" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT31" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU31" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV31" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW31" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX31" t="s">
         <v>46</v>
@@ -28327,7 +28329,7 @@
     </row>
     <row r="32" spans="1:52" ht="120">
       <c r="A32" s="1" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>955</v>
@@ -28342,7 +28344,7 @@
         <v>956</v>
       </c>
       <c r="F32" s="2">
-        <v>4077</v>
+        <v>4128</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>632</v>
@@ -28456,22 +28458,22 @@
         <v>987</v>
       </c>
       <c r="AR32" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS32" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT32" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU32" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV32" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW32" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX32" t="s">
         <v>46</v>
@@ -28485,7 +28487,7 @@
     </row>
     <row r="33" spans="1:52" ht="135">
       <c r="A33" s="1" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>988</v>
@@ -28614,22 +28616,22 @@
         <v>995</v>
       </c>
       <c r="AR33" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS33" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT33" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU33" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV33" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW33" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX33" t="s">
         <v>46</v>
@@ -28643,7 +28645,7 @@
     </row>
     <row r="34" spans="1:52" ht="135">
       <c r="A34" s="1" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>996</v>
@@ -28772,22 +28774,22 @@
         <v>1003</v>
       </c>
       <c r="AR34" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS34" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT34" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU34" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV34" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW34" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX34" t="s">
         <v>46</v>
@@ -28801,7 +28803,7 @@
     </row>
     <row r="35" spans="1:52" ht="135">
       <c r="A35" s="1" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>1004</v>
@@ -28930,22 +28932,22 @@
         <v>1011</v>
       </c>
       <c r="AR35" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS35" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT35" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU35" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV35" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW35" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX35" t="s">
         <v>46</v>
@@ -28959,7 +28961,7 @@
     </row>
     <row r="36" spans="1:52" ht="135">
       <c r="A36" s="1" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>1012</v>
@@ -29088,22 +29090,22 @@
         <v>1019</v>
       </c>
       <c r="AR36" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS36" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT36" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU36" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV36" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW36" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX36" t="s">
         <v>46</v>
@@ -29117,7 +29119,7 @@
     </row>
     <row r="37" spans="1:52" ht="150">
       <c r="A37" s="1" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>1020</v>
@@ -29246,22 +29248,22 @@
         <v>1027</v>
       </c>
       <c r="AR37" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS37" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT37" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU37" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV37" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW37" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX37" t="s">
         <v>46</v>
@@ -29275,7 +29277,7 @@
     </row>
     <row r="38" spans="1:52" ht="150">
       <c r="A38" s="17" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>298</v>
@@ -29404,22 +29406,22 @@
         <v>46</v>
       </c>
       <c r="AR38" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS38" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT38" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU38" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV38" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW38" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX38">
         <v>129</v>
@@ -29433,7 +29435,7 @@
     </row>
     <row r="39" spans="1:52" ht="90">
       <c r="A39" s="1" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>310</v>
@@ -29562,22 +29564,22 @@
         <v>333</v>
       </c>
       <c r="AR39" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS39" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT39" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU39" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV39" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW39" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX39">
         <v>401</v>
@@ -29591,7 +29593,7 @@
     </row>
     <row r="40" spans="1:52" ht="150">
       <c r="A40" s="1" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>1028</v>
@@ -29720,22 +29722,22 @@
         <v>1035</v>
       </c>
       <c r="AR40" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS40" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT40" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU40" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV40" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW40" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX40" t="s">
         <v>46</v>
@@ -29749,7 +29751,7 @@
     </row>
     <row r="41" spans="1:52" ht="150">
       <c r="A41" s="1" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>1039</v>
@@ -29878,22 +29880,22 @@
         <v>1054</v>
       </c>
       <c r="AR41" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS41" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT41" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU41" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV41" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW41" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX41" t="s">
         <v>46</v>
@@ -29907,7 +29909,7 @@
     </row>
     <row r="42" spans="1:52" ht="150">
       <c r="A42" s="1" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>1047</v>
@@ -30036,22 +30038,22 @@
         <v>1057</v>
       </c>
       <c r="AR42" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS42" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT42" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU42" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV42" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW42" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX42" t="s">
         <v>46</v>
@@ -30065,7 +30067,7 @@
     </row>
     <row r="43" spans="1:52" ht="150">
       <c r="A43" s="1" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>1053</v>
@@ -30194,22 +30196,22 @@
         <v>1067</v>
       </c>
       <c r="AR43" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS43" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT43" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU43" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV43" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW43" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX43" t="s">
         <v>46</v>
@@ -30223,7 +30225,7 @@
     </row>
     <row r="44" spans="1:52" ht="150">
       <c r="A44" s="1" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>1068</v>
@@ -30352,22 +30354,22 @@
         <v>1077</v>
       </c>
       <c r="AR44" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS44" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT44" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU44" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV44" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW44" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX44" t="s">
         <v>46</v>
@@ -30381,7 +30383,7 @@
     </row>
     <row r="45" spans="1:52" ht="150">
       <c r="A45" s="1" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>1078</v>
@@ -30510,22 +30512,22 @@
         <v>1086</v>
       </c>
       <c r="AR45" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS45" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT45" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU45" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV45" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW45" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX45" t="s">
         <v>46</v>
@@ -30539,7 +30541,7 @@
     </row>
     <row r="46" spans="1:52" ht="150">
       <c r="A46" s="1" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>1087</v>
@@ -30668,22 +30670,22 @@
         <v>1095</v>
       </c>
       <c r="AR46" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS46" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT46" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU46" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV46" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW46" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX46" t="s">
         <v>46</v>
@@ -30697,7 +30699,7 @@
     </row>
     <row r="47" spans="1:52" ht="150">
       <c r="A47" s="1" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>1096</v>
@@ -30826,22 +30828,22 @@
         <v>1104</v>
       </c>
       <c r="AR47" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS47" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT47" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU47" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV47" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW47" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX47" t="s">
         <v>46</v>
@@ -30855,7 +30857,7 @@
     </row>
     <row r="48" spans="1:52" ht="150">
       <c r="A48" s="1" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>1105</v>
@@ -30984,22 +30986,22 @@
         <v>1113</v>
       </c>
       <c r="AR48" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS48" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT48" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU48" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV48" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW48" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX48" t="s">
         <v>46</v>
@@ -31013,7 +31015,7 @@
     </row>
     <row r="49" spans="1:52" ht="90" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>47</v>
@@ -31142,22 +31144,22 @@
         <v>46</v>
       </c>
       <c r="AR49" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS49" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT49" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU49" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV49" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW49" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX49">
         <v>431</v>
@@ -31171,7 +31173,7 @@
     </row>
     <row r="50" spans="1:52" ht="75" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>335</v>
@@ -31300,22 +31302,22 @@
         <v>46</v>
       </c>
       <c r="AR50" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS50" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT50" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU50" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV50" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW50" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX50">
         <v>829</v>
@@ -31329,7 +31331,7 @@
     </row>
     <row r="51" spans="1:52" ht="120" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>350</v>
@@ -31368,7 +31370,7 @@
         <v>46</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="O51" s="2" t="s">
         <v>354</v>
@@ -31458,22 +31460,22 @@
         <v>46</v>
       </c>
       <c r="AR51" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS51" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT51" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU51" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV51" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW51" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX51">
         <v>106</v>
@@ -31487,7 +31489,7 @@
     </row>
     <row r="52" spans="1:52" ht="210" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>369</v>
@@ -31616,22 +31618,22 @@
         <v>46</v>
       </c>
       <c r="AR52" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS52" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT52" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU52" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV52" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW52" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX52">
         <v>92</v>
@@ -31645,7 +31647,7 @@
     </row>
     <row r="53" spans="1:52" ht="120" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>385</v>
@@ -31774,22 +31776,22 @@
         <v>46</v>
       </c>
       <c r="AR53" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS53" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT53" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU53" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV53" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW53" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX53">
         <v>5333</v>
@@ -31803,7 +31805,7 @@
     </row>
     <row r="54" spans="1:52" ht="180" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>406</v>
@@ -31932,22 +31934,22 @@
         <v>46</v>
       </c>
       <c r="AR54" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS54" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT54" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU54" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV54" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW54" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX54">
         <v>28</v>
@@ -31961,7 +31963,7 @@
     </row>
     <row r="55" spans="1:52" ht="180">
       <c r="A55" s="1" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>437</v>
@@ -32090,22 +32092,22 @@
         <v>46</v>
       </c>
       <c r="AR55" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS55" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT55" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU55" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AV55" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW55" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX55" t="s">
         <v>46</v>
@@ -32119,7 +32121,7 @@
     </row>
     <row r="56" spans="1:52" ht="75">
       <c r="A56" s="1" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>419</v>
@@ -32248,22 +32250,22 @@
         <v>46</v>
       </c>
       <c r="AR56" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS56" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT56" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU56" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV56" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW56" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX56">
         <v>185</v>
@@ -32277,10 +32279,10 @@
     </row>
     <row r="57" spans="1:52" ht="225">
       <c r="A57" s="21" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>1381</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>1382</v>
       </c>
       <c r="C57" s="2">
         <v>2021</v>
@@ -32289,16 +32291,16 @@
         <v>48</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="F57" s="23">
         <v>171</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>115</v>
@@ -32310,13 +32312,13 @@
         <v>658</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="M57" s="2" t="s">
         <v>110</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="O57" s="24">
         <v>0.54900000000000004</v>
@@ -32325,64 +32327,64 @@
         <v>46</v>
       </c>
       <c r="Q57" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="R57" s="2" t="s">
         <v>1423</v>
       </c>
-      <c r="R57" s="2" t="s">
+      <c r="S57" s="2" t="s">
         <v>1424</v>
-      </c>
-      <c r="S57" s="2" t="s">
-        <v>1425</v>
       </c>
       <c r="T57" s="2" t="s">
         <v>322</v>
       </c>
       <c r="U57" s="2" t="s">
+        <v>1384</v>
+      </c>
+      <c r="V57" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="W57" s="2" t="s">
         <v>1385</v>
       </c>
-      <c r="V57" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="W57" s="2" t="s">
+      <c r="X57" s="2" t="s">
         <v>1386</v>
       </c>
-      <c r="X57" s="2" t="s">
+      <c r="Y57" s="2" t="s">
         <v>1387</v>
-      </c>
-      <c r="Y57" s="2" t="s">
-        <v>1388</v>
       </c>
       <c r="Z57" s="2" t="s">
         <v>110</v>
       </c>
       <c r="AA57" s="2" t="s">
+        <v>1388</v>
+      </c>
+      <c r="AB57" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="AC57" s="2" t="s">
+        <v>1426</v>
+      </c>
+      <c r="AD57" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="AE57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH57" s="18" t="s">
+        <v>1428</v>
+      </c>
+      <c r="AI57" s="18" t="s">
+        <v>1429</v>
+      </c>
+      <c r="AJ57" s="2" t="s">
         <v>1389</v>
-      </c>
-      <c r="AB57" s="2" t="s">
-        <v>1426</v>
-      </c>
-      <c r="AC57" s="2" t="s">
-        <v>1427</v>
-      </c>
-      <c r="AD57" s="2" t="s">
-        <v>1428</v>
-      </c>
-      <c r="AE57" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF57" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG57" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH57" s="18" t="s">
-        <v>1429</v>
-      </c>
-      <c r="AI57" s="18" t="s">
-        <v>1430</v>
-      </c>
-      <c r="AJ57" s="2" t="s">
-        <v>1390</v>
       </c>
       <c r="AK57" s="2" t="s">
         <v>46</v>
@@ -32397,31 +32399,31 @@
         <v>0</v>
       </c>
       <c r="AO57" s="2" t="s">
+        <v>1430</v>
+      </c>
+      <c r="AP57" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="AQ57" s="2" t="s">
         <v>1431</v>
       </c>
-      <c r="AP57" s="2" t="s">
-        <v>1374</v>
-      </c>
-      <c r="AQ57" s="2" t="s">
-        <v>1432</v>
-      </c>
       <c r="AR57" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS57" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT57" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU57" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV57" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW57" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX57">
         <v>171</v>
@@ -32435,10 +32437,10 @@
     </row>
     <row r="58" spans="1:52" ht="165">
       <c r="A58" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="C58" s="2">
         <v>2021</v>
@@ -32453,7 +32455,7 @@
         <v>567</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>31</v>
@@ -32462,37 +32464,37 @@
         <v>29</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="K58" s="2" t="s">
         <v>658</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="M58" s="2" t="s">
         <v>110</v>
       </c>
       <c r="N58" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="O58" s="24" t="s">
+        <v>1456</v>
+      </c>
+      <c r="P58" s="2" t="s">
         <v>1394</v>
       </c>
-      <c r="O58" s="24" t="s">
-        <v>1435</v>
-      </c>
-      <c r="P58" s="2" t="s">
+      <c r="Q58" s="2" t="s">
         <v>1395</v>
       </c>
-      <c r="Q58" s="2" t="s">
+      <c r="R58" s="2" t="s">
+        <v>1386</v>
+      </c>
+      <c r="S58" s="2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="T58" s="2" t="s">
         <v>1396</v>
-      </c>
-      <c r="R58" s="2" t="s">
-        <v>1387</v>
-      </c>
-      <c r="S58" s="2" t="s">
-        <v>1436</v>
-      </c>
-      <c r="T58" s="2" t="s">
-        <v>1397</v>
       </c>
       <c r="U58" s="2" t="s">
         <v>746</v>
@@ -32501,10 +32503,10 @@
         <v>285</v>
       </c>
       <c r="W58" s="2" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="X58" s="2" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="Y58" s="2" t="s">
         <v>46</v>
@@ -32513,34 +32515,34 @@
         <v>110</v>
       </c>
       <c r="AA58" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="AB58" s="2" t="s">
         <v>1399</v>
       </c>
-      <c r="AB58" s="2" t="s">
+      <c r="AC58" s="2" t="s">
         <v>1400</v>
       </c>
-      <c r="AC58" s="2" t="s">
+      <c r="AD58" s="2" t="s">
         <v>1401</v>
       </c>
-      <c r="AD58" s="2" t="s">
+      <c r="AE58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH58" s="3" t="s">
         <v>1402</v>
       </c>
-      <c r="AE58" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF58" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG58" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH58" s="3" t="s">
+      <c r="AI58" s="18" t="s">
+        <v>1435</v>
+      </c>
+      <c r="AJ58" s="2" t="s">
         <v>1403</v>
-      </c>
-      <c r="AI58" s="18" t="s">
-        <v>1437</v>
-      </c>
-      <c r="AJ58" s="2" t="s">
-        <v>1404</v>
       </c>
       <c r="AK58" s="2" t="s">
         <v>46</v>
@@ -32555,31 +32557,31 @@
         <v>334</v>
       </c>
       <c r="AO58" s="2" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="AP58" s="2" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="AQ58" s="2" t="s">
         <v>334</v>
       </c>
       <c r="AR58" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS58" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT58" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU58" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV58" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW58" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX58">
         <v>567</v>
@@ -32593,7 +32595,7 @@
     </row>
     <row r="59" spans="1:52" ht="195">
       <c r="A59" s="1" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>82</v>
@@ -32680,7 +32682,7 @@
         <v>211</v>
       </c>
       <c r="AD59" s="2" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="AE59" s="2" t="s">
         <v>46</v>
@@ -32722,22 +32724,22 @@
         <v>46</v>
       </c>
       <c r="AR59" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS59" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT59" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU59" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV59" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW59" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX59">
         <v>87</v>
@@ -32751,7 +32753,7 @@
     </row>
     <row r="60" spans="1:52" ht="135">
       <c r="A60" s="1" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>446</v>
@@ -32880,22 +32882,22 @@
         <v>463</v>
       </c>
       <c r="AR60" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS60" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT60" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU60" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV60" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW60" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX60">
         <v>30896</v>
@@ -32909,7 +32911,7 @@
     </row>
     <row r="61" spans="1:52" ht="210">
       <c r="A61" s="1" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>464</v>
@@ -33038,22 +33040,22 @@
         <v>46</v>
       </c>
       <c r="AR61" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS61" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT61" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU61" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AV61" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW61" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX61">
         <v>91</v>
@@ -33067,7 +33069,7 @@
     </row>
     <row r="62" spans="1:52" ht="150">
       <c r="A62" s="1" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>483</v>
@@ -33196,22 +33198,22 @@
         <v>502</v>
       </c>
       <c r="AR62" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS62" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT62" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU62" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV62" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW62" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX62">
         <v>186</v>
@@ -33225,7 +33227,7 @@
     </row>
     <row r="63" spans="1:52" ht="105">
       <c r="A63" s="17" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>1221</v>
@@ -33361,22 +33363,22 @@
         <v>46</v>
       </c>
       <c r="AR63" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS63" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT63" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU63" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV63" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW63" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX63" t="s">
         <v>46</v>
@@ -33390,7 +33392,7 @@
     </row>
     <row r="64" spans="1:52" ht="120">
       <c r="A64" s="1" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>99</v>
@@ -33519,22 +33521,22 @@
         <v>46</v>
       </c>
       <c r="AR64" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS64" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT64" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU64" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV64" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW64" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX64">
         <v>139</v>
@@ -33548,7 +33550,7 @@
     </row>
     <row r="65" spans="1:52" ht="150">
       <c r="A65" s="1" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>503</v>
@@ -33677,22 +33679,22 @@
         <v>46</v>
       </c>
       <c r="AR65" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS65" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT65" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU65" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV65" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW65" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX65">
         <v>37</v>
@@ -33706,7 +33708,7 @@
     </row>
     <row r="66" spans="1:52" ht="105">
       <c r="A66" s="1" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>514</v>
@@ -33835,22 +33837,22 @@
         <v>46</v>
       </c>
       <c r="AR66" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS66" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT66" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU66" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV66" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW66" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX66">
         <v>986</v>
@@ -33864,7 +33866,7 @@
     </row>
     <row r="67" spans="1:52" ht="75">
       <c r="A67" s="1" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>531</v>
@@ -33993,22 +33995,22 @@
         <v>46</v>
       </c>
       <c r="AR67" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS67" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT67" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU67" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV67" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW67" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX67">
         <v>54</v>
@@ -34022,7 +34024,7 @@
     </row>
     <row r="68" spans="1:52" ht="75">
       <c r="A68" s="1" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>543</v>
@@ -34151,22 +34153,22 @@
         <v>557</v>
       </c>
       <c r="AR68" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS68" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT68" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU68" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV68" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW68" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX68">
         <v>354</v>
@@ -34180,7 +34182,7 @@
     </row>
     <row r="69" spans="1:52" ht="105">
       <c r="A69" s="1" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>558</v>
@@ -34309,22 +34311,22 @@
         <v>46</v>
       </c>
       <c r="AR69" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS69" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT69" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU69" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV69" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW69" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX69">
         <v>385</v>
@@ -34338,7 +34340,7 @@
     </row>
     <row r="70" spans="1:52" ht="105">
       <c r="A70" s="1" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>572</v>
@@ -34467,22 +34469,22 @@
         <v>46</v>
       </c>
       <c r="AR70" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS70" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT70" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU70" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV70" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW70" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX70">
         <v>487</v>
@@ -34496,7 +34498,7 @@
     </row>
     <row r="71" spans="1:52" ht="135">
       <c r="A71" s="1" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>586</v>
@@ -34625,22 +34627,22 @@
         <v>46</v>
       </c>
       <c r="AR71" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS71" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT71" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU71" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV71" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW71" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX71">
         <v>210</v>
@@ -34654,7 +34656,7 @@
     </row>
     <row r="72" spans="1:52" ht="120">
       <c r="A72" s="1" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>594</v>
@@ -34783,22 +34785,22 @@
         <v>46</v>
       </c>
       <c r="AR72" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS72" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT72" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU72" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV72" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW72" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX72">
         <v>198</v>
@@ -34812,7 +34814,7 @@
     </row>
     <row r="73" spans="1:52" ht="105">
       <c r="A73" s="1" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>608</v>
@@ -34830,7 +34832,7 @@
         <v>1270</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>31</v>
@@ -34941,22 +34943,22 @@
         <v>629</v>
       </c>
       <c r="AR73" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS73" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT73" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU73" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV73" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW73" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX73">
         <v>1270</v>
@@ -34970,7 +34972,7 @@
     </row>
     <row r="74" spans="1:52" ht="135">
       <c r="A74" s="1" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>630</v>
@@ -35099,22 +35101,22 @@
         <v>651</v>
       </c>
       <c r="AR74" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS74" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT74" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AU74" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV74" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW74" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX74" t="s">
         <v>46</v>
@@ -35128,7 +35130,7 @@
     </row>
     <row r="75" spans="1:52" ht="90">
       <c r="A75" s="1" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>652</v>
@@ -35167,46 +35169,46 @@
         <v>46</v>
       </c>
       <c r="N75" s="2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="O75" s="2" t="s">
         <v>1256</v>
       </c>
-      <c r="O75" s="2" t="s">
+      <c r="P75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U75" s="2" t="s">
         <v>1257</v>
       </c>
-      <c r="P75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="R75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="T75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="U75" s="2" t="s">
+      <c r="V75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W75" s="2" t="s">
         <v>1258</v>
       </c>
-      <c r="V75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="W75" s="2" t="s">
+      <c r="X75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z75" s="2" t="s">
         <v>1259</v>
       </c>
-      <c r="X75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z75" s="2" t="s">
+      <c r="AA75" s="2" t="s">
         <v>1260</v>
-      </c>
-      <c r="AA75" s="2" t="s">
-        <v>1261</v>
       </c>
       <c r="AB75" s="2">
         <v>4</v>
@@ -35215,10 +35217,10 @@
         <v>2</v>
       </c>
       <c r="AD75" s="2" t="s">
+        <v>1261</v>
+      </c>
+      <c r="AE75" s="3" t="s">
         <v>1262</v>
-      </c>
-      <c r="AE75" s="3" t="s">
-        <v>1263</v>
       </c>
       <c r="AF75" s="2" t="s">
         <v>46</v>
@@ -35257,22 +35259,22 @@
         <v>46</v>
       </c>
       <c r="AR75" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS75" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT75" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU75" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV75" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW75" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX75" t="s">
         <v>46</v>
@@ -35286,7 +35288,7 @@
     </row>
     <row r="76" spans="1:52" ht="135">
       <c r="A76" s="1" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>113</v>
@@ -35415,22 +35417,22 @@
         <v>46</v>
       </c>
       <c r="AR76" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS76" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT76" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU76" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV76" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW76" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX76">
         <v>1582</v>
@@ -35444,7 +35446,7 @@
     </row>
     <row r="77" spans="1:52" ht="150">
       <c r="A77" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>656</v>
@@ -35573,22 +35575,22 @@
         <v>46</v>
       </c>
       <c r="AR77" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS77" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT77" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU77" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV77" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW77" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX77" t="s">
         <v>46</v>
@@ -35602,7 +35604,7 @@
     </row>
     <row r="78" spans="1:52" ht="90">
       <c r="A78" s="1" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>64</v>
@@ -35701,7 +35703,7 @@
         <v>46</v>
       </c>
       <c r="AH78" s="15" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="AI78" s="3" t="s">
         <v>46</v>
@@ -35731,22 +35733,22 @@
         <v>81</v>
       </c>
       <c r="AR78" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS78" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT78" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU78" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV78" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW78" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX78">
         <v>130</v>
@@ -35760,10 +35762,10 @@
     </row>
     <row r="79" spans="1:52" ht="81.75" customHeight="1">
       <c r="A79" s="21" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="C79" s="2">
         <v>2018</v>
@@ -35772,19 +35774,19 @@
         <v>48</v>
       </c>
       <c r="E79" s="23" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="F79" s="2">
         <v>124</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>31</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>574</v>
@@ -35793,13 +35795,13 @@
         <v>658</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="M79" s="2" t="s">
         <v>110</v>
       </c>
       <c r="N79" s="23" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="O79" s="20">
         <v>0.47</v>
@@ -35817,7 +35819,7 @@
         <v>46</v>
       </c>
       <c r="T79" s="2" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="U79" s="2" t="s">
         <v>746</v>
@@ -35826,7 +35828,7 @@
         <v>46</v>
       </c>
       <c r="W79" s="2" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="X79" s="2" t="s">
         <v>602</v>
@@ -35835,19 +35837,19 @@
         <v>46</v>
       </c>
       <c r="Z79" s="2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="AA79" s="2" t="s">
+        <v>1416</v>
+      </c>
+      <c r="AB79" s="2" t="s">
+        <v>1376</v>
+      </c>
+      <c r="AC79" s="19" t="s">
+        <v>1377</v>
+      </c>
+      <c r="AD79" s="2" t="s">
         <v>1418</v>
-      </c>
-      <c r="AA79" s="2" t="s">
-        <v>1417</v>
-      </c>
-      <c r="AB79" s="2" t="s">
-        <v>1377</v>
-      </c>
-      <c r="AC79" s="19" t="s">
-        <v>1378</v>
-      </c>
-      <c r="AD79" s="2" t="s">
-        <v>1419</v>
       </c>
       <c r="AE79" s="2" t="s">
         <v>46</v>
@@ -35859,13 +35861,13 @@
         <v>46</v>
       </c>
       <c r="AH79" s="3" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="AI79" s="3" t="s">
         <v>46</v>
       </c>
       <c r="AJ79" s="2" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="AK79" s="2" t="s">
         <v>46</v>
@@ -35883,28 +35885,28 @@
         <v>334</v>
       </c>
       <c r="AP79" s="2" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="AQ79" s="2" t="s">
         <v>334</v>
       </c>
       <c r="AR79" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS79" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT79" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU79" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV79" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW79" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX79">
         <v>124</v>
@@ -35918,7 +35920,7 @@
     </row>
     <row r="80" spans="1:52" ht="90">
       <c r="A80" s="1" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>669</v>
@@ -36047,22 +36049,22 @@
         <v>46</v>
       </c>
       <c r="AR80" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS80" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT80" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU80" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV80" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW80" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AX80">
         <v>7122</v>
@@ -36076,7 +36078,7 @@
     </row>
     <row r="81" spans="1:52" ht="135">
       <c r="A81" s="1" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>678</v>
@@ -36205,22 +36207,22 @@
         <v>46</v>
       </c>
       <c r="AR81" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS81" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AT81" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU81" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV81" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW81" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX81">
         <v>296</v>
@@ -36234,7 +36236,7 @@
     </row>
     <row r="82" spans="1:52" ht="45">
       <c r="A82" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>699</v>
@@ -36363,22 +36365,22 @@
         <v>46</v>
       </c>
       <c r="AR82" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS82" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT82" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU82" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV82" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW82" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX82">
         <v>233</v>
@@ -36392,7 +36394,7 @@
     </row>
     <row r="83" spans="1:52" ht="75">
       <c r="A83" s="1" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>1236</v>
@@ -36491,26 +36493,26 @@
         <v>46</v>
       </c>
       <c r="AH83" s="3" t="s">
+        <v>1455</v>
+      </c>
+      <c r="AI83" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ83" s="2" t="s">
         <v>1250</v>
       </c>
-      <c r="AI83" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ83" s="2" t="s">
+      <c r="AK83" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL83" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM83" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN83" s="2" t="s">
         <v>1251</v>
       </c>
-      <c r="AK83" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL83" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM83" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN83" s="2" t="s">
-        <v>1252</v>
-      </c>
       <c r="AO83" s="2" t="s">
         <v>46</v>
       </c>
@@ -36521,22 +36523,22 @@
         <v>46</v>
       </c>
       <c r="AR83" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS83" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT83" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU83" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV83" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW83" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX83">
         <v>372</v>
@@ -36550,7 +36552,7 @@
     </row>
     <row r="84" spans="1:52" ht="90">
       <c r="A84" s="1" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>1114</v>
@@ -36679,22 +36681,22 @@
         <v>46</v>
       </c>
       <c r="AR84" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS84" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT84" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU84" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV84" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW84" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX84" t="s">
         <v>46</v>
@@ -36708,7 +36710,7 @@
     </row>
     <row r="85" spans="1:52" ht="90">
       <c r="A85" s="1" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>1115</v>
@@ -36837,22 +36839,22 @@
         <v>46</v>
       </c>
       <c r="AR85" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS85" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT85" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU85" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV85" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW85" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX85" t="s">
         <v>46</v>
@@ -36866,7 +36868,7 @@
     </row>
     <row r="86" spans="1:52" ht="90">
       <c r="A86" s="1" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>1116</v>
@@ -36995,22 +36997,22 @@
         <v>46</v>
       </c>
       <c r="AR86" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS86" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT86" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU86" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV86" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW86" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX86" t="s">
         <v>46</v>
@@ -37024,7 +37026,7 @@
     </row>
     <row r="87" spans="1:52" ht="165">
       <c r="A87" s="1" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>1117</v>
@@ -37153,22 +37155,22 @@
         <v>46</v>
       </c>
       <c r="AR87" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS87" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT87" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU87" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV87" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW87" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX87" t="s">
         <v>46</v>
@@ -37182,7 +37184,7 @@
     </row>
     <row r="88" spans="1:52" ht="90">
       <c r="A88" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>1153</v>
@@ -37311,22 +37313,22 @@
         <v>46</v>
       </c>
       <c r="AR88" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS88" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT88" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU88" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV88" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW88" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX88" t="s">
         <v>46</v>
@@ -37340,7 +37342,7 @@
     </row>
     <row r="89" spans="1:52" ht="105">
       <c r="A89" s="1" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>1162</v>
@@ -37469,22 +37471,22 @@
         <v>46</v>
       </c>
       <c r="AR89" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS89" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT89" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU89" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV89" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW89" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX89" t="s">
         <v>46</v>
@@ -37498,7 +37500,7 @@
     </row>
     <row r="90" spans="1:52" ht="105">
       <c r="A90" s="1" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>1171</v>
@@ -37627,22 +37629,22 @@
         <v>46</v>
       </c>
       <c r="AR90" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS90" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT90" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU90" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV90" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW90" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX90" t="s">
         <v>46</v>
@@ -37656,7 +37658,7 @@
     </row>
     <row r="91" spans="1:52" ht="105">
       <c r="A91" s="1" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>1180</v>
@@ -37785,22 +37787,22 @@
         <v>46</v>
       </c>
       <c r="AR91" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS91" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT91" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU91" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV91" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW91" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX91" t="s">
         <v>46</v>
@@ -37814,7 +37816,7 @@
     </row>
     <row r="92" spans="1:52" ht="90">
       <c r="A92" s="1" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>1189</v>
@@ -37943,22 +37945,22 @@
         <v>46</v>
       </c>
       <c r="AR92" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS92" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT92" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU92" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV92" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW92" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX92" t="s">
         <v>46</v>
@@ -37972,7 +37974,7 @@
     </row>
     <row r="93" spans="1:52" ht="147.94999999999999" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>1198</v>
@@ -38101,22 +38103,22 @@
         <v>46</v>
       </c>
       <c r="AR93" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS93" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT93" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU93" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV93" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW93" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX93" t="s">
         <v>46</v>
@@ -38130,7 +38132,7 @@
     </row>
     <row r="94" spans="1:52" ht="75">
       <c r="A94" s="1" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>712</v>
@@ -38259,22 +38261,22 @@
         <v>46</v>
       </c>
       <c r="AR94" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS94" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT94" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU94" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV94" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW94" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX94" t="s">
         <v>46</v>
@@ -38288,7 +38290,7 @@
     </row>
     <row r="95" spans="1:52" ht="315">
       <c r="A95" s="1" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>723</v>
@@ -38417,22 +38419,22 @@
         <v>736</v>
       </c>
       <c r="AR95" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AS95" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT95" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU95" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV95" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AW95" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX95" t="s">
         <v>46</v>
@@ -38446,7 +38448,7 @@
     </row>
     <row r="96" spans="1:52" ht="60">
       <c r="A96" s="1" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>737</v>
@@ -38575,22 +38577,22 @@
         <v>46</v>
       </c>
       <c r="AR96" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="AS96" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AT96" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AU96" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AV96" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AW96" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="AX96">
         <v>99</v>
@@ -38603,7 +38605,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A1:AQ96" xr:uid="{765A25C5-43E9-47DC-8427-7637ACFB5824}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AQ96">
       <sortCondition ref="A1:A96"/>

</xml_diff>

<commit_message>
Updated errors in analysis dataset and SR extraction data
</commit_message>
<xml_diff>
--- a/input/20220120-study.characteristics_update.xlsx
+++ b/input/20220120-study.characteristics_update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\SR_prevalence_NTM\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4549D0D-F9FB-49B7-9E2F-AF762C37BC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0B3AED-5755-4C7D-A896-59E41B603394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{9BAFF895-4EE1-48C5-B0C9-C001584A386E}"/>
   </bookViews>
@@ -22845,7 +22845,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23382,11 +23382,13 @@
   <dimension ref="A1:AZ96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.140625" style="2" customWidth="1"/>
@@ -23429,7 +23431,7 @@
     <col min="44" max="16384" width="18.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="20.25" customHeight="1">
+    <row r="1" spans="1:52" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1357</v>
       </c>
@@ -23587,7 +23589,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="158.25" customHeight="1">
+    <row r="2" spans="1:52" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1437</v>
       </c>
@@ -23745,7 +23747,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="120">
+    <row r="3" spans="1:52" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>1358</v>
       </c>
@@ -23903,7 +23905,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="269.25" customHeight="1">
+    <row r="4" spans="1:52" ht="269.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1270</v>
       </c>
@@ -24061,7 +24063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="240">
+    <row r="5" spans="1:52" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1271</v>
       </c>
@@ -24219,7 +24221,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="90">
+    <row r="6" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1272</v>
       </c>
@@ -24377,7 +24379,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="105">
+    <row r="7" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>1273</v>
       </c>
@@ -24535,7 +24537,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="150">
+    <row r="8" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1355</v>
       </c>
@@ -24693,7 +24695,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="150">
+    <row r="9" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1274</v>
       </c>
@@ -24851,7 +24853,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:52" ht="165">
+    <row r="10" spans="1:52" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1275</v>
       </c>
@@ -25009,7 +25011,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:52" ht="180">
+    <row r="11" spans="1:52" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1276</v>
       </c>
@@ -25167,7 +25169,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="225">
+    <row r="12" spans="1:52" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1277</v>
       </c>
@@ -25325,7 +25327,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:52" ht="240">
+    <row r="13" spans="1:52" ht="240" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1278</v>
       </c>
@@ -25483,7 +25485,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:52" ht="240">
+    <row r="14" spans="1:52" ht="240" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1279</v>
       </c>
@@ -25641,7 +25643,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:52" ht="240">
+    <row r="15" spans="1:52" ht="240" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1280</v>
       </c>
@@ -25799,7 +25801,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="240">
+    <row r="16" spans="1:52" ht="240" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1281</v>
       </c>
@@ -25957,7 +25959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:52" ht="60">
+    <row r="17" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1282</v>
       </c>
@@ -26115,7 +26117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:52" ht="270">
+    <row r="18" spans="1:52" ht="270" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>1283</v>
       </c>
@@ -26273,7 +26275,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:52" ht="180">
+    <row r="19" spans="1:52" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1284</v>
       </c>
@@ -26431,7 +26433,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:52" ht="120">
+    <row r="20" spans="1:52" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1285</v>
       </c>
@@ -26589,7 +26591,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:52" ht="120">
+    <row r="21" spans="1:52" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1286</v>
       </c>
@@ -26747,7 +26749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:52" ht="165">
+    <row r="22" spans="1:52" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>1287</v>
       </c>
@@ -26905,7 +26907,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:52" ht="210">
+    <row r="23" spans="1:52" ht="210" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1288</v>
       </c>
@@ -27063,7 +27065,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:52" ht="195">
+    <row r="24" spans="1:52" ht="195" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1289</v>
       </c>
@@ -27221,7 +27223,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:52" ht="180">
+    <row r="25" spans="1:52" ht="180" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1290</v>
       </c>
@@ -27379,7 +27381,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:52" ht="150">
+    <row r="26" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>1291</v>
       </c>
@@ -27537,7 +27539,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:52" ht="165">
+    <row r="27" spans="1:52" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1292</v>
       </c>
@@ -27695,7 +27697,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:52" ht="330">
+    <row r="28" spans="1:52" ht="330" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>1293</v>
       </c>
@@ -27853,7 +27855,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:52" ht="105">
+    <row r="29" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>1294</v>
       </c>
@@ -28011,7 +28013,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:52" ht="195">
+    <row r="30" spans="1:52" ht="195" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>1295</v>
       </c>
@@ -28169,7 +28171,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:52" ht="195">
+    <row r="31" spans="1:52" ht="195" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>1296</v>
       </c>
@@ -28327,7 +28329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:52" ht="120">
+    <row r="32" spans="1:52" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>1297</v>
       </c>
@@ -28485,7 +28487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:52" ht="135">
+    <row r="33" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>1298</v>
       </c>
@@ -28643,7 +28645,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:52" ht="135">
+    <row r="34" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1299</v>
       </c>
@@ -28801,7 +28803,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:52" ht="135">
+    <row r="35" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1300</v>
       </c>
@@ -28959,7 +28961,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:52" ht="135">
+    <row r="36" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1301</v>
       </c>
@@ -29117,7 +29119,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:52" ht="150">
+    <row r="37" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>1302</v>
       </c>
@@ -29275,7 +29277,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:52" ht="150">
+    <row r="38" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>1303</v>
       </c>
@@ -29433,7 +29435,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:52" ht="90">
+    <row r="39" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>1304</v>
       </c>
@@ -29591,7 +29593,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:52" ht="150">
+    <row r="40" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>1305</v>
       </c>
@@ -29749,7 +29751,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:52" ht="150">
+    <row r="41" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>1306</v>
       </c>
@@ -29907,7 +29909,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:52" ht="150">
+    <row r="42" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>1307</v>
       </c>
@@ -30065,7 +30067,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:52" ht="150">
+    <row r="43" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>1308</v>
       </c>
@@ -30223,7 +30225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:52" ht="150">
+    <row r="44" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>1309</v>
       </c>
@@ -30381,7 +30383,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:52" ht="150">
+    <row r="45" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>1310</v>
       </c>
@@ -30539,7 +30541,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:52" ht="150">
+    <row r="46" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>1311</v>
       </c>
@@ -30697,7 +30699,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:52" ht="150">
+    <row r="47" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>1312</v>
       </c>
@@ -30855,7 +30857,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:52" ht="150">
+    <row r="48" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>1313</v>
       </c>
@@ -31013,7 +31015,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:52" ht="90" customHeight="1">
+    <row r="49" spans="1:52" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>1439</v>
       </c>
@@ -31171,7 +31173,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="50" spans="1:52" ht="75" customHeight="1">
+    <row r="50" spans="1:52" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>1314</v>
       </c>
@@ -31329,7 +31331,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:52" ht="120" customHeight="1">
+    <row r="51" spans="1:52" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>1356</v>
       </c>
@@ -31487,7 +31489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:52" ht="210" customHeight="1">
+    <row r="52" spans="1:52" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>1350</v>
       </c>
@@ -31645,7 +31647,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:52" ht="120" customHeight="1">
+    <row r="53" spans="1:52" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>1438</v>
       </c>
@@ -31803,7 +31805,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:52" ht="180" customHeight="1">
+    <row r="54" spans="1:52" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>1315</v>
       </c>
@@ -31961,7 +31963,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:52" ht="180">
+    <row r="55" spans="1:52" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>1316</v>
       </c>
@@ -32119,7 +32121,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:52" ht="75">
+    <row r="56" spans="1:52" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>1351</v>
       </c>
@@ -32277,7 +32279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:52" ht="225">
+    <row r="57" spans="1:52" ht="225" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>1380</v>
       </c>
@@ -32435,7 +32437,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:52" ht="165">
+    <row r="58" spans="1:52" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>1390</v>
       </c>
@@ -32593,7 +32595,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:52" ht="195">
+    <row r="59" spans="1:52" ht="195" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>1352</v>
       </c>
@@ -32751,7 +32753,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:52" ht="135">
+    <row r="60" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>1317</v>
       </c>
@@ -32909,7 +32911,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:52" ht="210">
+    <row r="61" spans="1:52" ht="210" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>1318</v>
       </c>
@@ -33067,7 +33069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:52" ht="150">
+    <row r="62" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>1319</v>
       </c>
@@ -33225,7 +33227,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:52" ht="105">
+    <row r="63" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>1353</v>
       </c>
@@ -33390,7 +33392,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:52" ht="120">
+    <row r="64" spans="1:52" ht="120" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>1320</v>
       </c>
@@ -33548,7 +33550,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:52" ht="150">
+    <row r="65" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>1321</v>
       </c>
@@ -33706,7 +33708,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:52" ht="105">
+    <row r="66" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>1322</v>
       </c>
@@ -33864,7 +33866,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:52" ht="75">
+    <row r="67" spans="1:52" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>1323</v>
       </c>
@@ -34022,7 +34024,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:52" ht="75">
+    <row r="68" spans="1:52" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>1324</v>
       </c>
@@ -34180,7 +34182,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:52" ht="105">
+    <row r="69" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>1325</v>
       </c>
@@ -34338,7 +34340,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:52" ht="105">
+    <row r="70" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>1326</v>
       </c>
@@ -34496,7 +34498,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:52" ht="135">
+    <row r="71" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>1327</v>
       </c>
@@ -34654,7 +34656,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:52" ht="120">
+    <row r="72" spans="1:52" ht="120" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>1328</v>
       </c>
@@ -34812,7 +34814,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:52" ht="105">
+    <row r="73" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>1329</v>
       </c>
@@ -34970,7 +34972,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:52" ht="135">
+    <row r="74" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>1330</v>
       </c>
@@ -35128,7 +35130,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:52" ht="90">
+    <row r="75" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>1331</v>
       </c>
@@ -35286,7 +35288,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:52" ht="135">
+    <row r="76" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>1332</v>
       </c>
@@ -35444,7 +35446,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:52" ht="150">
+    <row r="77" spans="1:52" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>1333</v>
       </c>
@@ -35602,7 +35604,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:52" ht="90">
+    <row r="78" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>1334</v>
       </c>
@@ -35760,7 +35762,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:52" ht="81.75" customHeight="1">
+    <row r="79" spans="1:52" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
         <v>1411</v>
       </c>
@@ -35918,7 +35920,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:52" ht="90">
+    <row r="80" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>1335</v>
       </c>
@@ -36076,7 +36078,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:52" ht="135">
+    <row r="81" spans="1:52" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>1336</v>
       </c>
@@ -36234,7 +36236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:52" ht="45">
+    <row r="82" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>1269</v>
       </c>
@@ -36392,7 +36394,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:52" ht="75">
+    <row r="83" spans="1:52" ht="75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>1354</v>
       </c>
@@ -36550,7 +36552,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:52" ht="90">
+    <row r="84" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>1337</v>
       </c>
@@ -36708,7 +36710,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:52" ht="90">
+    <row r="85" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>1338</v>
       </c>
@@ -36866,7 +36868,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:52" ht="90">
+    <row r="86" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>1339</v>
       </c>
@@ -37024,7 +37026,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="1:52" ht="165">
+    <row r="87" spans="1:52" ht="165" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>1340</v>
       </c>
@@ -37182,7 +37184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="1:52" ht="90">
+    <row r="88" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>1341</v>
       </c>
@@ -37340,7 +37342,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="1:52" ht="105">
+    <row r="89" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>1342</v>
       </c>
@@ -37498,7 +37500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="90" spans="1:52" ht="105">
+    <row r="90" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>1343</v>
       </c>
@@ -37656,7 +37658,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="91" spans="1:52" ht="105">
+    <row r="91" spans="1:52" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>1344</v>
       </c>
@@ -37814,7 +37816,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:52" ht="90">
+    <row r="92" spans="1:52" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>1345</v>
       </c>
@@ -37972,7 +37974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="93" spans="1:52" ht="147.94999999999999" customHeight="1">
+    <row r="93" spans="1:52" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>1346</v>
       </c>
@@ -38130,7 +38132,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:52" ht="75">
+    <row r="94" spans="1:52" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>1347</v>
       </c>
@@ -38288,7 +38290,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:52" ht="315">
+    <row r="95" spans="1:52" ht="315" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>1348</v>
       </c>
@@ -38446,7 +38448,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="1:52" ht="60">
+    <row r="96" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>1349</v>
       </c>

</xml_diff>